<commit_message>
working on decision trees
</commit_message>
<xml_diff>
--- a/programs/frameworks/neural/data/dt.xlsx
+++ b/programs/frameworks/neural/data/dt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\objec\Documents\Code\objeck-lang\programs\frameworks\neural\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6061A9E9-6338-4842-A5C6-132CA9E79682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF42FE3-4877-4728-8E4D-9F0B23AE0680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11772" yWindow="1800" windowWidth="19272" windowHeight="13236" activeTab="1" xr2:uid="{8BC73549-3858-4843-9CB0-34D9690DEA20}"/>
+    <workbookView xWindow="11772" yWindow="1800" windowWidth="19272" windowHeight="13236" xr2:uid="{8BC73549-3858-4843-9CB0-34D9690DEA20}"/>
   </bookViews>
   <sheets>
     <sheet name="Perf" sheetId="1" r:id="rId1"/>
@@ -48,15 +48,9 @@
     <t>Class</t>
   </si>
   <si>
-    <t>Left target</t>
-  </si>
-  <si>
     <t>Left met</t>
   </si>
   <si>
-    <t>Right target</t>
-  </si>
-  <si>
     <t>Right met</t>
   </si>
   <si>
@@ -76,6 +70,12 @@
   </si>
   <si>
     <t>Parent</t>
+  </si>
+  <si>
+    <t>Left not met</t>
+  </si>
+  <si>
+    <t>Right not met</t>
   </si>
 </sst>
 </file>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A74A6F-E1C6-4FE1-9AA1-B58FD95A66B2}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,7 +468,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F1">
         <f>COUNTIFS(C2:C21,"&lt;&gt;"&amp;"")</f>
@@ -501,16 +501,16 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -550,7 +550,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <f>COUNTIFS(B2:B21, "TRUE",C2:C21, "TRUE")</f>
@@ -583,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <f>COUNTIF(B2:B21, "FALSE")</f>
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <f>COUNTIFS(B2:B21, "false",C2:C21, "TRUE")</f>
@@ -642,7 +642,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <f>F4/F1*H4+F7/F1*H7</f>
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C05382B-9C72-4B56-B866-4CD74987F803}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F1">
         <f>COUNTIFS(C2:C21,"&lt;&gt;"&amp;"")</f>
@@ -837,16 +837,16 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <f>COUNTIFS(B2:B21, "TRUE",C2:C21, "TRUE")</f>
@@ -918,7 +918,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -943,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <f>COUNTIFS(B2:B21, "false",C2:C21, "TRUE")</f>
@@ -976,7 +976,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <f>F4/F1*H4+F7/F1*H7</f>

</xml_diff>

<commit_message>
decision tree matrix, updates to csv library
</commit_message>
<xml_diff>
--- a/programs/frameworks/neural/data/dt.xlsx
+++ b/programs/frameworks/neural/data/dt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\objec\Documents\Code\objeck-lang\programs\frameworks\neural\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944DA1EB-1221-4FCE-9ABB-B5F182E7E468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1B6216-FB8A-4912-8476-D91C06BB1181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11136" yWindow="2148" windowWidth="21696" windowHeight="13236" xr2:uid="{8BC73549-3858-4843-9CB0-34D9690DEA20}"/>
   </bookViews>
@@ -99,8 +99,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -164,8 +172,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -527,7 +536,7 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="N27" sqref="N27:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,759 +555,766 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="17" t="s">
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="10"/>
+      <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
+      <c r="A2" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
     </row>
     <row r="3" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="B3" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" t="s">
+      <c r="A3" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="5">
         <f>COUNTIFS(C:C,"&lt;&gt;"&amp;"") -1</f>
         <v>20</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4"/>
+      <c r="A4" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5"/>
       <c r="K4" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="4" t="b">
+      <c r="L4" s="5" t="b">
         <f>(L5+L7)=$L$3</f>
         <v>1</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="B5" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="A5" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="7">
         <f>COUNTIF(B:B,"true")</f>
         <v>14</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="7">
         <f>L6/L5</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="6">
         <f>1-(M5*M5+M6*M6)</f>
         <v>0.48979591836734693</v>
       </c>
-      <c r="O5" s="12">
+      <c r="O5" s="13">
         <f>L5/$L$3*N5 + L7/$L$3*N7</f>
         <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="B6" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="6" t="s">
+      <c r="A6" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="7">
         <f>COUNTIFS(B:B,TRUE,C:C, "TRUE")</f>
         <v>8</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="7">
         <f>1-M5</f>
         <v>0.4285714285714286</v>
       </c>
-      <c r="N6" s="7"/>
-      <c r="O6" s="12"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="13"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="B7" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="5" t="s">
+      <c r="A7" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="7">
         <f>COUNTIF(B:B,"false")</f>
         <v>6</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="7">
         <f>L8/L7</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="6">
         <f>1-(M7*M7+M8*M8)</f>
         <v>0.44444444444444442</v>
       </c>
-      <c r="O7" s="12"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="B8" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="6" t="s">
+      <c r="A8" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="7">
         <f>COUNTIFS(B:B,FALSE,C:C, "TRUE")</f>
         <v>2</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="7">
         <f>1-M7</f>
         <v>0.66666666666666674</v>
       </c>
-      <c r="N8" s="7"/>
-      <c r="O8" s="12"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="13"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="B9" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+      <c r="A9" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="B10" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" s="4"/>
+      <c r="A10" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5"/>
       <c r="K10" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="4" t="b">
+      <c r="L10" s="5" t="b">
         <f>(L11+L13)=$L$3</f>
         <v>1</v>
       </c>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="B11" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="A11" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="K11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="7">
         <f>COUNTIF(A:A,"true")</f>
         <v>10</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="7">
         <f>L12/L11</f>
         <v>0.8</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="6">
         <f>1-(M11*M11+M12*M12)</f>
         <v>0.31999999999999984</v>
       </c>
-      <c r="O11" s="13">
+      <c r="O11" s="14">
         <f>L11/$L$3*N11 + L13/$L$3*N13</f>
         <v>0.31999999999999984</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6" t="s">
+      <c r="A12" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="7">
         <f>COUNTIFS(A:A,TRUE,C:C, "TRUE")</f>
         <v>8</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="7">
         <f>1-M11</f>
         <v>0.19999999999999996</v>
       </c>
-      <c r="N12" s="7"/>
-      <c r="O12" s="13"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="14"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="5" t="s">
+      <c r="A13" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="K13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="7">
         <f>COUNTIF(A:A,"false")</f>
         <v>10</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="7">
         <f>L14/L13</f>
         <v>0.2</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="6">
         <f>1-(M13*M13+M14*M14)</f>
         <v>0.31999999999999984</v>
       </c>
-      <c r="O13" s="13"/>
+      <c r="O13" s="14"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="B14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6" t="s">
+      <c r="A14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="7">
         <f>COUNTIFS(A:A,FALSE,C:C, "TRUE")</f>
         <v>2</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="7">
         <f>1-M13</f>
         <v>0.8</v>
       </c>
-      <c r="N14" s="7"/>
-      <c r="O14" s="13"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="14"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="B15" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="11"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="7"/>
+      <c r="A15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="8"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="B16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="A16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="5">
         <f>COUNTIFS(G:G,"&lt;&gt;"&amp;"") -1</f>
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="4"/>
+      <c r="A17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5"/>
       <c r="K17" t="s">
         <v>13</v>
       </c>
-      <c r="L17" s="4" t="b">
+      <c r="L17" s="5" t="b">
         <f>(L18+L20)=$L$16</f>
         <v>1</v>
       </c>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
     </row>
     <row r="18" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="3" t="s">
+      <c r="A18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="7">
         <f>COUNTIF(F:F,"true")</f>
         <v>8</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="7">
         <f>L19/L18</f>
         <v>1</v>
       </c>
-      <c r="N18" s="7">
+      <c r="N18" s="6">
         <f>1-(M18*M18+M19*M19)</f>
         <v>0</v>
       </c>
-      <c r="O18" s="16">
+      <c r="O18" s="17">
         <f>L18/$L$3*N18 + L20/$L$3*N20</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="B19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6" t="s">
+      <c r="A19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="7">
         <f>COUNTIFS(F:F,TRUE,G:G, "TRUE")</f>
         <v>8</v>
       </c>
-      <c r="M19" s="6">
+      <c r="M19" s="7">
         <f>1-M18</f>
         <v>0</v>
       </c>
-      <c r="N19" s="7"/>
-      <c r="O19" s="16"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="17"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="B20" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="5" t="s">
+      <c r="A20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="K20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="6">
+      <c r="L20" s="7">
         <f>COUNTIF(F:F,"false")</f>
         <v>2</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="7">
         <f>L21/L20</f>
         <v>1</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="6">
         <f>1-(M20*M20+M21*M21)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="16"/>
+      <c r="O20" s="17"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6" t="s">
+      <c r="A21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="6">
+      <c r="L21" s="7">
         <f>COUNTIFS(F:F,FALSE,G:G, "TRUE")</f>
         <v>2</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="7">
         <f>1-M20</f>
         <v>0</v>
       </c>
-      <c r="N21" s="7"/>
-      <c r="O21" s="16"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="17"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="K23" t="s">
         <v>12</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="5">
         <f>COUNTIFS(G:G,"&lt;&gt;"&amp;"") -1</f>
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="J24" s="4"/>
+      <c r="J24" s="5"/>
       <c r="K24" t="s">
         <v>13</v>
       </c>
-      <c r="L24" s="4" t="b">
+      <c r="L24" s="5" t="b">
         <f>(L25+L27)=$L$16</f>
         <v>1</v>
       </c>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
     </row>
     <row r="25" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="J25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K25" s="6" t="s">
+      <c r="K25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L25" s="6">
+      <c r="L25" s="7">
         <f>COUNTIF(E:E,"true")</f>
         <v>8</v>
       </c>
-      <c r="M25" s="6">
+      <c r="M25" s="7">
         <f>L26/L25</f>
         <v>1</v>
       </c>
-      <c r="N25" s="7">
+      <c r="N25" s="6">
         <f>1-(M25*M25+M26*M26)</f>
         <v>0</v>
       </c>
-      <c r="O25" s="16">
+      <c r="O25" s="17">
         <f>L25/$L$3*N25 + L27/$L$3*N27</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I26" s="3"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="6" t="s">
+      <c r="I26" s="4"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L26" s="6">
+      <c r="L26" s="7">
         <f>COUNTIFS(E:E,TRUE,G:G, "TRUE")</f>
         <v>8</v>
       </c>
-      <c r="M26" s="6">
+      <c r="M26" s="7">
         <f>1-M25</f>
         <v>0</v>
       </c>
-      <c r="N26" s="7"/>
-      <c r="O26" s="16"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="17"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I27" s="3"/>
-      <c r="J27" s="5" t="s">
+      <c r="I27" s="4"/>
+      <c r="J27" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="K27" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L27" s="6">
+      <c r="L27" s="7">
         <f>COUNTIF(E:E,"false")</f>
         <v>2</v>
       </c>
-      <c r="M27" s="6">
+      <c r="M27" s="7">
         <f>L28/L27</f>
         <v>1</v>
       </c>
-      <c r="N27" s="7">
+      <c r="N27" s="6">
         <f>1-(M27*M27+M28*M28)</f>
         <v>0</v>
       </c>
-      <c r="O27" s="16"/>
+      <c r="O27" s="17"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I28" s="3"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="6" t="s">
+      <c r="I28" s="4"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L28" s="6">
+      <c r="L28" s="7">
         <f>COUNTIFS(E:E,FALSE,G:G, "TRUE")</f>
         <v>2</v>
       </c>
-      <c r="M28" s="6">
+      <c r="M28" s="7">
         <f>1-M27</f>
         <v>0</v>
       </c>
-      <c r="N28" s="7"/>
-      <c r="O28" s="16"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="24">
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="N27:N28"/>
     <mergeCell ref="I25:I28"/>
     <mergeCell ref="J25:J26"/>
     <mergeCell ref="O25:O28"/>
     <mergeCell ref="J27:J28"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="N18:N19"/>
     <mergeCell ref="I11:I14"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="J13:J14"/>
@@ -1308,6 +1324,7 @@
     <mergeCell ref="J18:J19"/>
     <mergeCell ref="O18:O21"/>
     <mergeCell ref="J20:J21"/>
+    <mergeCell ref="N20:N21"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="I5:I8"/>

</xml_diff>